<commit_message>
1st sprint review protocol & mockup imgs
</commit_message>
<xml_diff>
--- a/documents/sprint/Sprint_Review_Protocol_Loot_Ledger_1.xlsx
+++ b/documents/sprint/Sprint_Review_Protocol_Loot_Ledger_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\itp-project\ITP-DnD-Itembar\documents\sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D02B8F-F24F-4903-A6B2-653C62C156E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DE27FA-326E-41AE-8186-4F57DB676C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Mock Ups für die einzelnen Seite erstellen</t>
+  </si>
+  <si>
+    <t>Pair programming</t>
   </si>
 </sst>
 </file>
@@ -379,17 +382,23 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -397,50 +406,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,14 +761,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE3C726-37E9-451B-9308-D99ECF6E7468}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="41.88671875" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
@@ -775,28 +778,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
@@ -810,10 +813,10 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="17">
         <v>1</v>
       </c>
@@ -823,120 +826,120 @@
       <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="29">
+      <c r="B5" s="16"/>
+      <c r="C5" s="19">
         <v>45384</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="19">
+      <c r="B6" s="16"/>
+      <c r="C6" s="20">
         <v>5</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="23" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="9" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="10"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="29"/>
+      <c r="C12" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -972,14 +975,18 @@
         <v>28</v>
       </c>
       <c r="C16" s="7">
-        <v>5</v>
-      </c>
-      <c r="D16" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="D16" s="7">
+        <v>10</v>
+      </c>
       <c r="E16" s="2">
-        <f t="shared" ref="E16:E25" si="0">D16-C16</f>
-        <v>-5</v>
-      </c>
-      <c r="F16" s="3"/>
+        <f t="shared" ref="E16:E20" si="0">D16-C16</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
       <c r="G16" s="4"/>
       <c r="H16" s="7"/>
     </row>
@@ -993,14 +1000,20 @@
       <c r="C17" s="7">
         <v>2</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="7">
+        <v>2</v>
+      </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-      <c r="F17" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
@@ -1013,13 +1026,15 @@
         <v>1</v>
       </c>
       <c r="D18" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>-0.5</v>
-      </c>
-      <c r="F18" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="7"/>
     </row>
@@ -1033,14 +1048,20 @@
       <c r="C19" s="7">
         <v>5</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="7">
+        <v>4</v>
+      </c>
       <c r="E19" s="2">
         <f t="shared" si="0"/>
-        <v>-5</v>
-      </c>
-      <c r="F19" s="3"/>
+        <v>-1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="7"/>
+      <c r="H19" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
@@ -1052,14 +1073,20 @@
       <c r="C20" s="7">
         <v>8</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="7">
+        <v>7</v>
+      </c>
       <c r="E20" s="2">
         <f t="shared" si="0"/>
-        <v>-8</v>
-      </c>
-      <c r="F20" s="3"/>
+        <v>-1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="7"/>
+      <c r="H20" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
@@ -1116,11 +1143,11 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6">
         <f>SUM(E16:E25)</f>
-        <v>-20.5</v>
+        <v>-2</v>
       </c>
       <c r="F26" s="6">
         <f>COUNT(F16:F25)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G26" s="6">
         <f>COUNT(G16:G25)</f>
@@ -1141,6 +1168,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
@@ -1157,12 +1188,11 @@
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="90" orientation="landscape" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="8" max="1048575" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
</xml_diff>